<commit_message>
added genes table and standardized names
</commit_message>
<xml_diff>
--- a/emx/cosas-refs/cosasrefs.xlsx
+++ b/emx/cosas-refs/cosasrefs.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="111">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -34,7 +34,7 @@
     <t xml:space="preserve">COSAS References</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference tables for COSAS (v0.91, 2021-07-08)</t>
+    <t xml:space="preserve">Reference tables for COSAS (v0.9002, 2021-07-09)</t>
   </si>
   <si>
     <t xml:space="preserve">label-nl</t>
@@ -118,6 +118,21 @@
     <t xml:space="preserve">Testcodes and beschrijvingen (bijv., NX, NG)</t>
   </si>
   <si>
+    <t xml:space="preserve">genes_by_test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Genes by test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Genen per test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">List of genes by test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lijst van genen per test</t>
+  </si>
+  <si>
     <t xml:space="preserve">lab_indications</t>
   </si>
   <si>
@@ -157,19 +172,22 @@
     <t xml:space="preserve">dataType</t>
   </si>
   <si>
+    <t xml:space="preserve">entity</t>
+  </si>
+  <si>
     <t xml:space="preserve">lookupAttribute</t>
   </si>
   <si>
-    <t xml:space="preserve">entity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">category</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Category</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Categorie</t>
+    <t xml:space="preserve">labelAttribute</t>
+  </si>
+  <si>
+    <t xml:space="preserve">refEntity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ID</t>
   </si>
   <si>
     <t xml:space="preserve">string</t>
@@ -178,7 +196,13 @@
     <t xml:space="preserve">cosasrefs_diagnostic_certainty</t>
   </si>
   <si>
-    <t xml:space="preserve">Label</t>
+    <t xml:space="preserve">certainty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Certainty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zekerheid</t>
   </si>
   <si>
     <t xml:space="preserve">Description</t>
@@ -187,63 +211,81 @@
     <t xml:space="preserve">Omschrijving</t>
   </si>
   <si>
-    <t xml:space="preserve">id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ID</t>
-  </si>
-  <si>
     <t xml:space="preserve">cosasrefs_diagnoses</t>
   </si>
   <si>
+    <t xml:space="preserve">cineas_code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CINEAS code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diagnostic code (e.g., 12345)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diagnostische code (bijv, 12345)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cineas_description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diagnosis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diagnose</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cosasrefs_material_types</t>
+  </si>
+  <si>
+    <t xml:space="preserve">material</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Material</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Materiaal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cosasrefs_condition_codes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Naam</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cosasrefs_test_codes</t>
+  </si>
+  <si>
     <t xml:space="preserve">code</t>
   </si>
   <si>
-    <t xml:space="preserve">Diagnosis code</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Diagnose code</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Diagnostic code (e.g., 12345)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Diagnostische code (bijv, 12345)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Diagnosis description</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Diagnose beschrijvingen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cosasrefs_material_types</t>
-  </si>
-  <si>
-    <t xml:space="preserve">type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Type</t>
-  </si>
-  <si>
     <t xml:space="preserve">Code</t>
   </si>
   <si>
-    <t xml:space="preserve">cosasrefs_condition_codes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Naam</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cosasrefs_test_codes</t>
-  </si>
-  <si>
     <t xml:space="preserve">Beschrijving</t>
   </si>
   <si>
+    <t xml:space="preserve">genes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Genes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mref</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cosasrefs_genes_by_test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test Code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Genen</t>
+  </si>
+  <si>
     <t xml:space="preserve">cosasrefs_lab_indications</t>
   </si>
   <si>
@@ -256,16 +298,13 @@
     <t xml:space="preserve">Indicatie</t>
   </si>
   <si>
+    <t xml:space="preserve">cosasrefs_phenotypic_sex</t>
+  </si>
+  <si>
     <t xml:space="preserve">value</t>
   </si>
   <si>
-    <t xml:space="preserve">Sex</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Geslacht</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cosasrefs_phenotypic_sex</t>
+    <t xml:space="preserve">COSAS Value</t>
   </si>
   <si>
     <t xml:space="preserve">codesystem</t>
@@ -283,6 +322,9 @@
     <t xml:space="preserve">vrouw</t>
   </si>
   <si>
+    <t xml:space="preserve">female</t>
+  </si>
+  <si>
     <t xml:space="preserve">A biological sex quality inhering in an individual or a population that only produces gametes that can be fertilised by male gametes.</t>
   </si>
   <si>
@@ -296,6 +338,9 @@
   </si>
   <si>
     <t xml:space="preserve">man</t>
+  </si>
+  <si>
+    <t xml:space="preserve">male</t>
   </si>
   <si>
     <t xml:space="preserve">A biological sex quality inhering in an individual or a population whose sex organs contain only male gametes.</t>
@@ -832,6 +877,26 @@
         <v>3</v>
       </c>
     </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C9" t="s">
+        <v>45</v>
+      </c>
+      <c r="D9" t="s">
+        <v>46</v>
+      </c>
+      <c r="E9" t="s">
+        <v>47</v>
+      </c>
+      <c r="F9" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
@@ -857,594 +922,814 @@
         <v>6</v>
       </c>
       <c r="D1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G1" t="s">
+        <v>51</v>
+      </c>
+      <c r="H1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="F1" t="s">
-        <v>43</v>
-      </c>
-      <c r="G1" t="s">
-        <v>44</v>
-      </c>
-      <c r="H1" t="s">
-        <v>45</v>
-      </c>
-      <c r="I1" t="s">
-        <v>46</v>
-      </c>
       <c r="J1" t="s">
-        <v>47</v>
+        <v>52</v>
+      </c>
+      <c r="K1" t="s">
+        <v>53</v>
+      </c>
+      <c r="L1" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="B2" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="C2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G2" t="b">
-        <v>0</v>
-      </c>
-      <c r="H2" t="s">
-        <v>51</v>
-      </c>
-      <c r="I2" t="b">
-        <v>1</v>
-      </c>
-      <c r="J2" t="s">
-        <v>52</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="D2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F2" t="s">
+        <v>57</v>
+      </c>
+      <c r="G2" t="s">
+        <v>58</v>
+      </c>
+      <c r="H2"/>
+      <c r="I2"/>
+      <c r="J2" t="b">
+        <v>0</v>
+      </c>
+      <c r="K2" t="b">
+        <v>0</v>
+      </c>
+      <c r="L2"/>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>59</v>
       </c>
       <c r="B3" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="C3" t="s">
-        <v>53</v>
-      </c>
-      <c r="D3"/>
-      <c r="E3"/>
-      <c r="F3" t="b">
-        <v>0</v>
-      </c>
-      <c r="G3" t="b">
-        <v>1</v>
+        <v>61</v>
+      </c>
+      <c r="D3" t="b">
+        <v>0</v>
+      </c>
+      <c r="E3" t="b">
+        <v>1</v>
+      </c>
+      <c r="F3" t="s">
+        <v>57</v>
+      </c>
+      <c r="G3" t="s">
+        <v>58</v>
       </c>
       <c r="H3" t="s">
-        <v>51</v>
-      </c>
-      <c r="I3" t="b">
-        <v>0</v>
-      </c>
-      <c r="J3" t="s">
-        <v>52</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="I3" t="s">
+        <v>11</v>
+      </c>
+      <c r="J3" t="b">
+        <v>1</v>
+      </c>
+      <c r="K3" t="b">
+        <v>1</v>
+      </c>
+      <c r="L3"/>
     </row>
     <row r="4">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="C4" t="s">
-        <v>55</v>
-      </c>
-      <c r="D4"/>
-      <c r="E4"/>
-      <c r="F4" t="b">
-        <v>0</v>
-      </c>
-      <c r="G4" t="b">
-        <v>1</v>
-      </c>
-      <c r="H4" t="s">
-        <v>51</v>
-      </c>
-      <c r="I4" t="b">
-        <v>0</v>
-      </c>
-      <c r="J4" t="s">
-        <v>52</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="D4" t="b">
+        <v>0</v>
+      </c>
+      <c r="E4" t="b">
+        <v>1</v>
+      </c>
+      <c r="F4" t="s">
+        <v>57</v>
+      </c>
+      <c r="G4" t="s">
+        <v>58</v>
+      </c>
+      <c r="H4"/>
+      <c r="I4"/>
+      <c r="J4" t="b">
+        <v>0</v>
+      </c>
+      <c r="K4" t="b">
+        <v>0</v>
+      </c>
+      <c r="L4"/>
     </row>
     <row r="5">
       <c r="A5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B5" t="s">
         <v>56</v>
       </c>
-      <c r="B5" t="s">
-        <v>57</v>
-      </c>
       <c r="C5" t="s">
-        <v>57</v>
-      </c>
-      <c r="D5"/>
-      <c r="E5"/>
-      <c r="F5" t="b">
-        <v>1</v>
-      </c>
-      <c r="G5" t="b">
-        <v>0</v>
-      </c>
-      <c r="H5" t="s">
-        <v>51</v>
-      </c>
-      <c r="I5" t="b">
-        <v>0</v>
-      </c>
-      <c r="J5" t="s">
-        <v>58</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="D5" t="b">
+        <v>1</v>
+      </c>
+      <c r="E5" t="b">
+        <v>0</v>
+      </c>
+      <c r="F5" t="s">
+        <v>57</v>
+      </c>
+      <c r="G5" t="s">
+        <v>64</v>
+      </c>
+      <c r="H5"/>
+      <c r="I5"/>
+      <c r="J5" t="b">
+        <v>0</v>
+      </c>
+      <c r="K5" t="b">
+        <v>0</v>
+      </c>
+      <c r="L5"/>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="B6" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="C6" t="s">
-        <v>61</v>
-      </c>
-      <c r="D6" t="s">
-        <v>62</v>
-      </c>
-      <c r="E6" t="s">
-        <v>63</v>
-      </c>
-      <c r="F6" t="b">
-        <v>0</v>
-      </c>
-      <c r="G6" t="b">
-        <v>1</v>
+        <v>66</v>
+      </c>
+      <c r="D6" t="b">
+        <v>0</v>
+      </c>
+      <c r="E6" t="b">
+        <v>1</v>
+      </c>
+      <c r="F6" t="s">
+        <v>57</v>
+      </c>
+      <c r="G6" t="s">
+        <v>64</v>
       </c>
       <c r="H6" t="s">
-        <v>51</v>
-      </c>
-      <c r="I6" t="b">
-        <v>1</v>
-      </c>
-      <c r="J6" t="s">
-        <v>58</v>
-      </c>
+        <v>67</v>
+      </c>
+      <c r="I6" t="s">
+        <v>68</v>
+      </c>
+      <c r="J6" t="b">
+        <v>1</v>
+      </c>
+      <c r="K6" t="b">
+        <v>1</v>
+      </c>
+      <c r="L6"/>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>2</v>
+        <v>69</v>
       </c>
       <c r="B7" t="s">
+        <v>70</v>
+      </c>
+      <c r="C7" t="s">
+        <v>71</v>
+      </c>
+      <c r="D7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F7" t="s">
+        <v>57</v>
+      </c>
+      <c r="G7" t="s">
         <v>64</v>
       </c>
-      <c r="C7" t="s">
-        <v>65</v>
-      </c>
-      <c r="D7"/>
-      <c r="E7"/>
-      <c r="F7" t="b">
-        <v>0</v>
-      </c>
-      <c r="G7" t="b">
-        <v>1</v>
-      </c>
-      <c r="H7" t="s">
-        <v>51</v>
-      </c>
-      <c r="I7" t="b">
-        <v>0</v>
-      </c>
-      <c r="J7" t="s">
-        <v>58</v>
-      </c>
+      <c r="H7"/>
+      <c r="I7"/>
+      <c r="J7" t="b">
+        <v>0</v>
+      </c>
+      <c r="K7" t="b">
+        <v>0</v>
+      </c>
+      <c r="L7"/>
     </row>
     <row r="8">
       <c r="A8" t="s">
+        <v>55</v>
+      </c>
+      <c r="B8" t="s">
         <v>56</v>
       </c>
-      <c r="B8" t="s">
-        <v>57</v>
-      </c>
       <c r="C8" t="s">
-        <v>57</v>
-      </c>
-      <c r="D8"/>
-      <c r="E8"/>
-      <c r="F8" t="b">
-        <v>1</v>
-      </c>
-      <c r="G8" t="b">
-        <v>0</v>
-      </c>
-      <c r="H8" t="s">
-        <v>51</v>
-      </c>
-      <c r="I8" t="b">
-        <v>1</v>
-      </c>
-      <c r="J8" t="s">
-        <v>66</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="D8" t="b">
+        <v>1</v>
+      </c>
+      <c r="E8" t="b">
+        <v>0</v>
+      </c>
+      <c r="F8" t="s">
+        <v>57</v>
+      </c>
+      <c r="G8" t="s">
+        <v>72</v>
+      </c>
+      <c r="H8"/>
+      <c r="I8"/>
+      <c r="J8" t="b">
+        <v>0</v>
+      </c>
+      <c r="K8" t="b">
+        <v>0</v>
+      </c>
+      <c r="L8"/>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="B9" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="C9" t="s">
-        <v>68</v>
-      </c>
-      <c r="D9"/>
-      <c r="E9"/>
-      <c r="F9" t="b">
-        <v>0</v>
-      </c>
-      <c r="G9" t="b">
-        <v>1</v>
-      </c>
-      <c r="H9" t="s">
-        <v>51</v>
-      </c>
-      <c r="I9" t="b">
-        <v>0</v>
-      </c>
-      <c r="J9" t="s">
-        <v>66</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="D9" t="b">
+        <v>0</v>
+      </c>
+      <c r="E9" t="b">
+        <v>1</v>
+      </c>
+      <c r="F9" t="s">
+        <v>57</v>
+      </c>
+      <c r="G9" t="s">
+        <v>72</v>
+      </c>
+      <c r="H9"/>
+      <c r="I9"/>
+      <c r="J9" t="b">
+        <v>1</v>
+      </c>
+      <c r="K9" t="b">
+        <v>1</v>
+      </c>
+      <c r="L9"/>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B10" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
       <c r="C10" t="s">
-        <v>69</v>
-      </c>
-      <c r="D10"/>
-      <c r="E10"/>
-      <c r="F10" t="b">
-        <v>1</v>
-      </c>
-      <c r="G10" t="b">
-        <v>0</v>
-      </c>
-      <c r="H10" t="s">
-        <v>51</v>
-      </c>
-      <c r="I10" t="b">
-        <v>1</v>
-      </c>
-      <c r="J10" t="s">
-        <v>70</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="D10" t="b">
+        <v>1</v>
+      </c>
+      <c r="E10" t="b">
+        <v>0</v>
+      </c>
+      <c r="F10" t="s">
+        <v>57</v>
+      </c>
+      <c r="G10" t="s">
+        <v>76</v>
+      </c>
+      <c r="H10"/>
+      <c r="I10"/>
+      <c r="J10" t="b">
+        <v>0</v>
+      </c>
+      <c r="K10" t="b">
+        <v>0</v>
+      </c>
+      <c r="L10"/>
     </row>
     <row r="11">
       <c r="A11" t="s">
         <v>0</v>
       </c>
       <c r="B11" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="C11" t="s">
-        <v>72</v>
-      </c>
-      <c r="D11"/>
-      <c r="E11"/>
-      <c r="F11" t="b">
-        <v>0</v>
-      </c>
-      <c r="G11" t="b">
-        <v>1</v>
-      </c>
-      <c r="H11" t="s">
-        <v>51</v>
-      </c>
-      <c r="I11" t="b">
-        <v>0</v>
-      </c>
-      <c r="J11" t="s">
-        <v>70</v>
-      </c>
+        <v>78</v>
+      </c>
+      <c r="D11" t="b">
+        <v>0</v>
+      </c>
+      <c r="E11" t="b">
+        <v>1</v>
+      </c>
+      <c r="F11" t="s">
+        <v>57</v>
+      </c>
+      <c r="G11" t="s">
+        <v>76</v>
+      </c>
+      <c r="H11"/>
+      <c r="I11"/>
+      <c r="J11" t="b">
+        <v>1</v>
+      </c>
+      <c r="K11" t="b">
+        <v>1</v>
+      </c>
+      <c r="L11"/>
     </row>
     <row r="12">
       <c r="A12" t="s">
+        <v>55</v>
+      </c>
+      <c r="B12" t="s">
         <v>56</v>
       </c>
-      <c r="B12" t="s">
-        <v>57</v>
-      </c>
       <c r="C12" t="s">
-        <v>57</v>
-      </c>
-      <c r="D12"/>
-      <c r="E12"/>
-      <c r="F12" t="b">
-        <v>1</v>
-      </c>
-      <c r="G12" t="b">
-        <v>0</v>
-      </c>
-      <c r="H12" t="s">
-        <v>51</v>
-      </c>
-      <c r="I12" t="b">
-        <v>1</v>
-      </c>
-      <c r="J12" t="s">
-        <v>73</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="D12" t="b">
+        <v>1</v>
+      </c>
+      <c r="E12" t="b">
+        <v>0</v>
+      </c>
+      <c r="F12" t="s">
+        <v>57</v>
+      </c>
+      <c r="G12" t="s">
+        <v>79</v>
+      </c>
+      <c r="H12"/>
+      <c r="I12"/>
+      <c r="J12" t="b">
+        <v>0</v>
+      </c>
+      <c r="K12" t="b">
+        <v>0</v>
+      </c>
+      <c r="L12"/>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>59</v>
+        <v>80</v>
       </c>
       <c r="B13" t="s">
-        <v>69</v>
+        <v>81</v>
       </c>
       <c r="C13" t="s">
-        <v>69</v>
-      </c>
-      <c r="D13"/>
-      <c r="E13"/>
-      <c r="F13" t="b">
-        <v>0</v>
-      </c>
-      <c r="G13" t="b">
-        <v>1</v>
-      </c>
-      <c r="H13" t="s">
-        <v>51</v>
-      </c>
-      <c r="I13" t="b">
-        <v>0</v>
-      </c>
-      <c r="J13" t="s">
-        <v>73</v>
-      </c>
+        <v>81</v>
+      </c>
+      <c r="D13" t="b">
+        <v>0</v>
+      </c>
+      <c r="E13" t="b">
+        <v>1</v>
+      </c>
+      <c r="F13" t="s">
+        <v>57</v>
+      </c>
+      <c r="G13" t="s">
+        <v>79</v>
+      </c>
+      <c r="H13"/>
+      <c r="I13"/>
+      <c r="J13" t="b">
+        <v>1</v>
+      </c>
+      <c r="K13" t="b">
+        <v>1</v>
+      </c>
+      <c r="L13"/>
     </row>
     <row r="14">
       <c r="A14" t="s">
         <v>2</v>
       </c>
       <c r="B14" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="C14" t="s">
-        <v>74</v>
-      </c>
-      <c r="D14"/>
-      <c r="E14"/>
-      <c r="F14" t="b">
-        <v>0</v>
-      </c>
-      <c r="G14" t="b">
-        <v>1</v>
-      </c>
-      <c r="H14" t="s">
-        <v>51</v>
-      </c>
-      <c r="I14" t="b">
-        <v>0</v>
-      </c>
-      <c r="J14" t="s">
-        <v>73</v>
-      </c>
+        <v>82</v>
+      </c>
+      <c r="D14" t="b">
+        <v>0</v>
+      </c>
+      <c r="E14" t="b">
+        <v>1</v>
+      </c>
+      <c r="F14" t="s">
+        <v>57</v>
+      </c>
+      <c r="G14" t="s">
+        <v>79</v>
+      </c>
+      <c r="H14"/>
+      <c r="I14"/>
+      <c r="J14" t="b">
+        <v>0</v>
+      </c>
+      <c r="K14" t="b">
+        <v>0</v>
+      </c>
+      <c r="L14"/>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>59</v>
+        <v>83</v>
       </c>
       <c r="B15" t="s">
-        <v>69</v>
+        <v>84</v>
       </c>
       <c r="C15" t="s">
-        <v>69</v>
-      </c>
-      <c r="D15"/>
-      <c r="E15"/>
-      <c r="F15" t="b">
-        <v>1</v>
-      </c>
-      <c r="G15" t="b">
-        <v>0</v>
-      </c>
-      <c r="H15" t="s">
-        <v>51</v>
-      </c>
-      <c r="I15" t="b">
-        <v>1</v>
-      </c>
-      <c r="J15" t="s">
-        <v>75</v>
+        <v>84</v>
+      </c>
+      <c r="D15" t="b">
+        <v>0</v>
+      </c>
+      <c r="E15" t="b">
+        <v>1</v>
+      </c>
+      <c r="F15" t="s">
+        <v>85</v>
+      </c>
+      <c r="G15" t="s">
+        <v>79</v>
+      </c>
+      <c r="H15"/>
+      <c r="I15"/>
+      <c r="J15" t="b">
+        <v>0</v>
+      </c>
+      <c r="K15" t="b">
+        <v>0</v>
+      </c>
+      <c r="L15" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>76</v>
+        <v>55</v>
       </c>
       <c r="B16" t="s">
-        <v>77</v>
+        <v>56</v>
       </c>
       <c r="C16" t="s">
-        <v>78</v>
-      </c>
-      <c r="D16"/>
-      <c r="E16"/>
-      <c r="F16" t="b">
-        <v>0</v>
-      </c>
-      <c r="G16" t="b">
-        <v>1</v>
+        <v>56</v>
+      </c>
+      <c r="D16" t="b">
+        <v>1</v>
+      </c>
+      <c r="E16" t="b">
+        <v>0</v>
+      </c>
+      <c r="F16" t="s">
+        <v>57</v>
+      </c>
+      <c r="G16" t="s">
+        <v>86</v>
       </c>
       <c r="H16" t="s">
-        <v>51</v>
-      </c>
-      <c r="I16" t="b">
-        <v>0</v>
-      </c>
-      <c r="J16" t="s">
-        <v>75</v>
-      </c>
+        <v>87</v>
+      </c>
+      <c r="I16" t="s">
+        <v>87</v>
+      </c>
+      <c r="J16" t="b">
+        <v>0</v>
+      </c>
+      <c r="K16" t="b">
+        <v>0</v>
+      </c>
+      <c r="L16"/>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="B17" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="C17" t="s">
-        <v>81</v>
-      </c>
-      <c r="D17"/>
-      <c r="E17"/>
-      <c r="F17" t="b">
-        <v>1</v>
-      </c>
-      <c r="G17" t="b">
-        <v>0</v>
-      </c>
-      <c r="H17" t="s">
-        <v>51</v>
-      </c>
-      <c r="I17" t="b">
-        <v>0</v>
-      </c>
-      <c r="J17" t="s">
-        <v>82</v>
-      </c>
+        <v>88</v>
+      </c>
+      <c r="D17" t="b">
+        <v>0</v>
+      </c>
+      <c r="E17" t="b">
+        <v>1</v>
+      </c>
+      <c r="F17" t="s">
+        <v>57</v>
+      </c>
+      <c r="G17" t="s">
+        <v>86</v>
+      </c>
+      <c r="H17"/>
+      <c r="I17"/>
+      <c r="J17" t="b">
+        <v>1</v>
+      </c>
+      <c r="K17" t="b">
+        <v>1</v>
+      </c>
+      <c r="L17"/>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>2</v>
+        <v>55</v>
       </c>
       <c r="B18" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C18" t="s">
-        <v>55</v>
-      </c>
-      <c r="D18"/>
-      <c r="E18"/>
-      <c r="F18" t="b">
-        <v>0</v>
-      </c>
-      <c r="G18" t="b">
-        <v>1</v>
-      </c>
-      <c r="H18" t="s">
-        <v>51</v>
-      </c>
-      <c r="I18" t="b">
-        <v>0</v>
-      </c>
-      <c r="J18" t="s">
-        <v>82</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="D18" t="b">
+        <v>1</v>
+      </c>
+      <c r="E18" t="b">
+        <v>0</v>
+      </c>
+      <c r="F18" t="s">
+        <v>57</v>
+      </c>
+      <c r="G18" t="s">
+        <v>89</v>
+      </c>
+      <c r="H18"/>
+      <c r="I18"/>
+      <c r="J18" t="b">
+        <v>0</v>
+      </c>
+      <c r="K18" t="b">
+        <v>0</v>
+      </c>
+      <c r="L18"/>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="B19" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
       <c r="C19" t="s">
-        <v>84</v>
-      </c>
-      <c r="D19"/>
-      <c r="E19"/>
-      <c r="F19" t="b">
-        <v>0</v>
-      </c>
-      <c r="G19" t="b">
-        <v>1</v>
-      </c>
-      <c r="H19" t="s">
-        <v>51</v>
-      </c>
-      <c r="I19" t="b">
-        <v>0</v>
-      </c>
-      <c r="J19" t="s">
-        <v>82</v>
-      </c>
+        <v>92</v>
+      </c>
+      <c r="D19" t="b">
+        <v>0</v>
+      </c>
+      <c r="E19" t="b">
+        <v>1</v>
+      </c>
+      <c r="F19" t="s">
+        <v>57</v>
+      </c>
+      <c r="G19" t="s">
+        <v>89</v>
+      </c>
+      <c r="H19"/>
+      <c r="I19"/>
+      <c r="J19" t="b">
+        <v>1</v>
+      </c>
+      <c r="K19" t="b">
+        <v>1</v>
+      </c>
+      <c r="L19"/>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B20" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
       <c r="C20" t="s">
-        <v>69</v>
-      </c>
-      <c r="D20"/>
-      <c r="E20"/>
-      <c r="F20" t="b">
-        <v>0</v>
-      </c>
-      <c r="G20" t="b">
-        <v>1</v>
-      </c>
-      <c r="H20" t="s">
-        <v>51</v>
-      </c>
-      <c r="I20" t="b">
-        <v>0</v>
-      </c>
-      <c r="J20" t="s">
-        <v>82</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="D20" t="b">
+        <v>1</v>
+      </c>
+      <c r="E20" t="b">
+        <v>0</v>
+      </c>
+      <c r="F20" t="s">
+        <v>57</v>
+      </c>
+      <c r="G20" t="s">
+        <v>93</v>
+      </c>
+      <c r="H20"/>
+      <c r="I20"/>
+      <c r="J20" t="b">
+        <v>1</v>
+      </c>
+      <c r="K20" t="b">
+        <v>1</v>
+      </c>
+      <c r="L20"/>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="B21" t="s">
-        <v>85</v>
+        <v>95</v>
       </c>
       <c r="C21" t="s">
-        <v>85</v>
-      </c>
-      <c r="D21"/>
-      <c r="E21"/>
-      <c r="F21" t="b">
-        <v>0</v>
-      </c>
-      <c r="G21" t="b">
-        <v>1</v>
-      </c>
-      <c r="H21" t="s">
-        <v>86</v>
-      </c>
-      <c r="I21" t="b">
-        <v>0</v>
-      </c>
-      <c r="J21" t="s">
-        <v>82</v>
-      </c>
+        <v>95</v>
+      </c>
+      <c r="D21" t="b">
+        <v>0</v>
+      </c>
+      <c r="E21" t="b">
+        <v>1</v>
+      </c>
+      <c r="F21" t="s">
+        <v>57</v>
+      </c>
+      <c r="G21" t="s">
+        <v>93</v>
+      </c>
+      <c r="H21"/>
+      <c r="I21"/>
+      <c r="J21" t="b">
+        <v>0</v>
+      </c>
+      <c r="K21" t="b">
+        <v>0</v>
+      </c>
+      <c r="L21"/>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>2</v>
+      </c>
+      <c r="B22" t="s">
+        <v>62</v>
+      </c>
+      <c r="C22" t="s">
+        <v>63</v>
+      </c>
+      <c r="D22" t="b">
+        <v>0</v>
+      </c>
+      <c r="E22" t="b">
+        <v>1</v>
+      </c>
+      <c r="F22" t="s">
+        <v>57</v>
+      </c>
+      <c r="G22" t="s">
+        <v>93</v>
+      </c>
+      <c r="H22"/>
+      <c r="I22"/>
+      <c r="J22" t="b">
+        <v>0</v>
+      </c>
+      <c r="K22" t="b">
+        <v>0</v>
+      </c>
+      <c r="L22"/>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>96</v>
+      </c>
+      <c r="B23" t="s">
+        <v>97</v>
+      </c>
+      <c r="C23" t="s">
+        <v>97</v>
+      </c>
+      <c r="D23" t="b">
+        <v>0</v>
+      </c>
+      <c r="E23" t="b">
+        <v>1</v>
+      </c>
+      <c r="F23" t="s">
+        <v>57</v>
+      </c>
+      <c r="G23" t="s">
+        <v>93</v>
+      </c>
+      <c r="H23"/>
+      <c r="I23"/>
+      <c r="J23" t="b">
+        <v>0</v>
+      </c>
+      <c r="K23" t="b">
+        <v>0</v>
+      </c>
+      <c r="L23"/>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>80</v>
+      </c>
+      <c r="B24" t="s">
+        <v>81</v>
+      </c>
+      <c r="C24" t="s">
+        <v>81</v>
+      </c>
+      <c r="D24" t="b">
+        <v>0</v>
+      </c>
+      <c r="E24" t="b">
+        <v>1</v>
+      </c>
+      <c r="F24" t="s">
+        <v>57</v>
+      </c>
+      <c r="G24" t="s">
+        <v>93</v>
+      </c>
+      <c r="H24"/>
+      <c r="I24"/>
+      <c r="J24" t="b">
+        <v>0</v>
+      </c>
+      <c r="K24" t="b">
+        <v>0</v>
+      </c>
+      <c r="L24"/>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>98</v>
+      </c>
+      <c r="B25" t="s">
+        <v>98</v>
+      </c>
+      <c r="C25" t="s">
+        <v>98</v>
+      </c>
+      <c r="D25" t="b">
+        <v>0</v>
+      </c>
+      <c r="E25" t="b">
+        <v>1</v>
+      </c>
+      <c r="F25" t="s">
+        <v>99</v>
+      </c>
+      <c r="G25" t="s">
+        <v>93</v>
+      </c>
+      <c r="H25"/>
+      <c r="I25"/>
+      <c r="J25" t="b">
+        <v>0</v>
+      </c>
+      <c r="K25" t="b">
+        <v>0</v>
+      </c>
+      <c r="L25"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1488,53 +1773,62 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>79</v>
+        <v>55</v>
       </c>
       <c r="B1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
-        <v>83</v>
-      </c>
       <c r="D1" t="s">
-        <v>59</v>
+        <v>96</v>
       </c>
       <c r="E1" t="s">
-        <v>85</v>
+        <v>80</v>
+      </c>
+      <c r="F1" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>87</v>
+        <v>100</v>
       </c>
       <c r="B2" t="s">
-        <v>88</v>
+        <v>101</v>
       </c>
       <c r="C2" t="s">
-        <v>89</v>
+        <v>102</v>
       </c>
       <c r="D2" t="s">
-        <v>90</v>
+        <v>103</v>
       </c>
       <c r="E2" t="s">
-        <v>91</v>
+        <v>104</v>
+      </c>
+      <c r="F2" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>92</v>
+        <v>106</v>
       </c>
       <c r="B3" t="s">
-        <v>93</v>
+        <v>107</v>
       </c>
       <c r="C3" t="s">
-        <v>89</v>
+        <v>108</v>
       </c>
       <c r="D3" t="s">
-        <v>94</v>
+        <v>103</v>
       </c>
       <c r="E3" t="s">
-        <v>95</v>
+        <v>109</v>
+      </c>
+      <c r="F3" t="s">
+        <v>110</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added genes ref entity, reset test codes
</commit_message>
<xml_diff>
--- a/emx/cosas-refs/cosasrefs.xlsx
+++ b/emx/cosas-refs/cosasrefs.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="111">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -34,7 +34,7 @@
     <t xml:space="preserve">COSAS References</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference tables for COSAS (v0.9003, 2021-07-12)</t>
+    <t xml:space="preserve">Reference tables for COSAS (v0.9004, 2021-07-13)</t>
   </si>
   <si>
     <t xml:space="preserve">label-nl</t>
@@ -46,6 +46,33 @@
     <t xml:space="preserve">package</t>
   </si>
   <si>
+    <t xml:space="preserve">condition_codes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Condition</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aandoening</t>
+  </si>
+  <si>
+    <t xml:space="preserve">General disease codes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aandoening codes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">diagnoses</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diagnoses</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diagnostic codes and descriptions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diagnostische codes en beschrijvingen</t>
+  </si>
+  <si>
     <t xml:space="preserve">diagnostic_certainty</t>
   </si>
   <si>
@@ -61,16 +88,19 @@
     <t xml:space="preserve">Categoriën voor diagnostisch zekerheid</t>
   </si>
   <si>
-    <t xml:space="preserve">diagnoses</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Diagnoses</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Diagnostic codes and descriptions</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Diagnostische codes en beschrijvingen</t>
+    <t xml:space="preserve">lab_indications</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lab Indications</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Labindicaties</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Categories for purpose of the labs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Categoriën voor het doel van de laboratia</t>
   </si>
   <si>
     <t xml:space="preserve">material_types</t>
@@ -88,19 +118,19 @@
     <t xml:space="preserve">Categoriën voor materiaaltype</t>
   </si>
   <si>
-    <t xml:space="preserve">condition_codes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Condition</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Aandoening</t>
-  </si>
-  <si>
-    <t xml:space="preserve">General disease codes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Aandoening codes</t>
+    <t xml:space="preserve">phenotypic_sex</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Phenotypic Sex</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Phenotypic Geslacht</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Categories for phenotypic sex</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Categoriën voor phenotypic geslacht</t>
   </si>
   <si>
     <t xml:space="preserve">test_codes</t>
@@ -118,34 +148,19 @@
     <t xml:space="preserve">Testcodes and beschrijvingen (bijv., NX, NG)</t>
   </si>
   <si>
-    <t xml:space="preserve">lab_indications</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lab Indications</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Labindicaties</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Categories for purpose of the labs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Categoriën voor het doel van de laboratia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">phenotypic_sex</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Phenotypic Sex</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Phenotypic Geslacht</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Categories for phenotypic sex</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Categoriën voor phenotypic geslacht</t>
+    <t xml:space="preserve">test_genes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gene List</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gene Lijst</t>
+  </si>
+  <si>
+    <t xml:space="preserve">List of genes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lijst van genen</t>
   </si>
   <si>
     <t xml:space="preserve">idAttribute</t>
@@ -175,6 +190,39 @@
     <t xml:space="preserve">string</t>
   </si>
   <si>
+    <t xml:space="preserve">cosasrefs_condition_codes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Naam</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cosasrefs_diagnoses</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cineas_code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CINEAS code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diagnostic code (e.g., 12345)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diagnostische code (bijv, 12345)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cineas_description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diagnosis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diagnose</t>
+  </si>
+  <si>
     <t xml:space="preserve">cosasrefs_diagnostic_certainty</t>
   </si>
   <si>
@@ -193,28 +241,16 @@
     <t xml:space="preserve">Omschrijving</t>
   </si>
   <si>
-    <t xml:space="preserve">cosasrefs_diagnoses</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cineas_code</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CINEAS code</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Diagnostic code (e.g., 12345)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Diagnostische code (bijv, 12345)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cineas_description</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Diagnosis</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Diagnose</t>
+    <t xml:space="preserve">cosasrefs_lab_indications</t>
+  </si>
+  <si>
+    <t xml:space="preserve">indication</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Indication</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Indicatie</t>
   </si>
   <si>
     <t xml:space="preserve">cosasrefs_material_types</t>
@@ -229,24 +265,36 @@
     <t xml:space="preserve">Materiaal</t>
   </si>
   <si>
-    <t xml:space="preserve">cosasrefs_condition_codes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Naam</t>
+    <t xml:space="preserve">cosasrefs_phenotypic_sex</t>
+  </si>
+  <si>
+    <t xml:space="preserve">value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">codesystem</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Code system</t>
+  </si>
+  <si>
+    <t xml:space="preserve">code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">iri</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hyperlink</t>
   </si>
   <si>
     <t xml:space="preserve">cosasrefs_test_codes</t>
   </si>
   <si>
-    <t xml:space="preserve">code</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Code</t>
-  </si>
-  <si>
     <t xml:space="preserve">Beschrijving</t>
   </si>
   <si>
@@ -259,37 +307,16 @@
     <t xml:space="preserve">text</t>
   </si>
   <si>
-    <t xml:space="preserve">cosasrefs_lab_indications</t>
-  </si>
-  <si>
-    <t xml:space="preserve">indication</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Indication</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Indicatie</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cosasrefs_phenotypic_sex</t>
-  </si>
-  <si>
-    <t xml:space="preserve">value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">codesystem</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Code system</t>
-  </si>
-  <si>
-    <t xml:space="preserve">iri</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hyperlink</t>
+    <t xml:space="preserve">gene</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gene</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cosasrefs_test_genes</t>
   </si>
   <si>
     <t xml:space="preserve">vrouw</t>
@@ -850,6 +877,26 @@
         <v>3</v>
       </c>
     </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C9" t="s">
+        <v>45</v>
+      </c>
+      <c r="D9" t="s">
+        <v>46</v>
+      </c>
+      <c r="E9" t="s">
+        <v>47</v>
+      </c>
+      <c r="F9" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
@@ -875,39 +922,39 @@
         <v>6</v>
       </c>
       <c r="D1" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="E1" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="F1" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="G1" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="H1" t="s">
+        <v>52</v>
+      </c>
+      <c r="I1" t="s">
+        <v>53</v>
+      </c>
+      <c r="J1" t="s">
         <v>2</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>7</v>
-      </c>
-      <c r="J1" t="s">
-        <v>47</v>
-      </c>
-      <c r="K1" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="B2" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="C2" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="D2" t="b">
         <v>1</v>
@@ -916,29 +963,29 @@
         <v>0</v>
       </c>
       <c r="F2" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="G2" t="s">
-        <v>52</v>
-      </c>
-      <c r="H2"/>
-      <c r="I2"/>
-      <c r="J2" t="b">
-        <v>0</v>
-      </c>
-      <c r="K2" t="b">
-        <v>0</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="H2" t="b">
+        <v>0</v>
+      </c>
+      <c r="I2" t="b">
+        <v>0</v>
+      </c>
+      <c r="J2"/>
+      <c r="K2"/>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>53</v>
+        <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="C3" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="D3" t="b">
         <v>0</v>
@@ -947,223 +994,223 @@
         <v>1</v>
       </c>
       <c r="F3" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="G3" t="s">
-        <v>52</v>
-      </c>
-      <c r="H3" t="s">
-        <v>10</v>
-      </c>
-      <c r="I3" t="s">
-        <v>11</v>
-      </c>
-      <c r="J3" t="b">
-        <v>1</v>
-      </c>
-      <c r="K3" t="b">
-        <v>1</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="H3" t="b">
+        <v>1</v>
+      </c>
+      <c r="I3" t="b">
+        <v>1</v>
+      </c>
+      <c r="J3"/>
+      <c r="K3"/>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>54</v>
       </c>
       <c r="B4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F4" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="G4" t="s">
-        <v>52</v>
-      </c>
-      <c r="H4"/>
-      <c r="I4"/>
-      <c r="J4" t="b">
-        <v>0</v>
-      </c>
-      <c r="K4" t="b">
-        <v>0</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="H4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I4" t="b">
+        <v>0</v>
+      </c>
+      <c r="J4"/>
+      <c r="K4"/>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="B5" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="C5" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="D5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F5" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="G5" t="s">
-        <v>58</v>
-      </c>
-      <c r="H5"/>
-      <c r="I5"/>
-      <c r="J5" t="b">
-        <v>0</v>
-      </c>
-      <c r="K5" t="b">
-        <v>0</v>
+        <v>60</v>
+      </c>
+      <c r="H5" t="b">
+        <v>1</v>
+      </c>
+      <c r="I5" t="b">
+        <v>1</v>
+      </c>
+      <c r="J5" t="s">
+        <v>63</v>
+      </c>
+      <c r="K5" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="B6" t="s">
+        <v>66</v>
+      </c>
+      <c r="C6" t="s">
+        <v>67</v>
+      </c>
+      <c r="D6" t="b">
+        <v>0</v>
+      </c>
+      <c r="E6" t="b">
+        <v>1</v>
+      </c>
+      <c r="F6" t="s">
+        <v>56</v>
+      </c>
+      <c r="G6" t="s">
         <v>60</v>
       </c>
-      <c r="C6" t="s">
-        <v>60</v>
-      </c>
-      <c r="D6" t="b">
-        <v>0</v>
-      </c>
-      <c r="E6" t="b">
-        <v>1</v>
-      </c>
-      <c r="F6" t="s">
-        <v>51</v>
-      </c>
-      <c r="G6" t="s">
-        <v>58</v>
-      </c>
-      <c r="H6" t="s">
-        <v>61</v>
-      </c>
-      <c r="I6" t="s">
-        <v>62</v>
-      </c>
-      <c r="J6" t="b">
-        <v>1</v>
-      </c>
-      <c r="K6" t="b">
-        <v>1</v>
-      </c>
+      <c r="H6" t="b">
+        <v>0</v>
+      </c>
+      <c r="I6" t="b">
+        <v>0</v>
+      </c>
+      <c r="J6"/>
+      <c r="K6"/>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="B7" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="C7" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="D7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F7" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="G7" t="s">
-        <v>58</v>
-      </c>
-      <c r="H7"/>
-      <c r="I7"/>
-      <c r="J7" t="b">
-        <v>0</v>
-      </c>
-      <c r="K7" t="b">
-        <v>0</v>
-      </c>
+        <v>68</v>
+      </c>
+      <c r="H7" t="b">
+        <v>0</v>
+      </c>
+      <c r="I7" t="b">
+        <v>0</v>
+      </c>
+      <c r="J7"/>
+      <c r="K7"/>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>49</v>
+        <v>69</v>
       </c>
       <c r="B8" t="s">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="C8" t="s">
-        <v>50</v>
+        <v>71</v>
       </c>
       <c r="D8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F8" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="G8" t="s">
-        <v>66</v>
-      </c>
-      <c r="H8"/>
-      <c r="I8"/>
-      <c r="J8" t="b">
-        <v>0</v>
-      </c>
-      <c r="K8" t="b">
-        <v>0</v>
+        <v>68</v>
+      </c>
+      <c r="H8" t="b">
+        <v>1</v>
+      </c>
+      <c r="I8" t="b">
+        <v>1</v>
+      </c>
+      <c r="J8" t="s">
+        <v>19</v>
+      </c>
+      <c r="K8" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>67</v>
+        <v>2</v>
       </c>
       <c r="B9" t="s">
+        <v>72</v>
+      </c>
+      <c r="C9" t="s">
+        <v>73</v>
+      </c>
+      <c r="D9" t="b">
+        <v>0</v>
+      </c>
+      <c r="E9" t="b">
+        <v>1</v>
+      </c>
+      <c r="F9" t="s">
+        <v>56</v>
+      </c>
+      <c r="G9" t="s">
         <v>68</v>
       </c>
-      <c r="C9" t="s">
-        <v>69</v>
-      </c>
-      <c r="D9" t="b">
-        <v>0</v>
-      </c>
-      <c r="E9" t="b">
-        <v>1</v>
-      </c>
-      <c r="F9" t="s">
-        <v>51</v>
-      </c>
-      <c r="G9" t="s">
-        <v>66</v>
-      </c>
-      <c r="H9"/>
-      <c r="I9"/>
-      <c r="J9" t="b">
-        <v>1</v>
-      </c>
-      <c r="K9" t="b">
-        <v>1</v>
-      </c>
+      <c r="H9" t="b">
+        <v>0</v>
+      </c>
+      <c r="I9" t="b">
+        <v>0</v>
+      </c>
+      <c r="J9"/>
+      <c r="K9"/>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="B10" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="C10" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="D10" t="b">
         <v>1</v>
@@ -1172,29 +1219,29 @@
         <v>0</v>
       </c>
       <c r="F10" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="G10" t="s">
-        <v>70</v>
-      </c>
-      <c r="H10"/>
-      <c r="I10"/>
-      <c r="J10" t="b">
-        <v>0</v>
-      </c>
-      <c r="K10" t="b">
-        <v>0</v>
-      </c>
+        <v>74</v>
+      </c>
+      <c r="H10" t="b">
+        <v>0</v>
+      </c>
+      <c r="I10" t="b">
+        <v>0</v>
+      </c>
+      <c r="J10"/>
+      <c r="K10"/>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="B11" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="C11" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="D11" t="b">
         <v>0</v>
@@ -1203,29 +1250,29 @@
         <v>1</v>
       </c>
       <c r="F11" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="G11" t="s">
-        <v>70</v>
-      </c>
-      <c r="H11"/>
-      <c r="I11"/>
-      <c r="J11" t="b">
-        <v>1</v>
-      </c>
-      <c r="K11" t="b">
-        <v>1</v>
-      </c>
+        <v>74</v>
+      </c>
+      <c r="H11" t="b">
+        <v>1</v>
+      </c>
+      <c r="I11" t="b">
+        <v>1</v>
+      </c>
+      <c r="J11"/>
+      <c r="K11"/>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="B12" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="C12" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="D12" t="b">
         <v>1</v>
@@ -1234,29 +1281,29 @@
         <v>0</v>
       </c>
       <c r="F12" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="G12" t="s">
-        <v>73</v>
-      </c>
-      <c r="H12"/>
-      <c r="I12"/>
-      <c r="J12" t="b">
-        <v>0</v>
-      </c>
-      <c r="K12" t="b">
-        <v>0</v>
-      </c>
+        <v>78</v>
+      </c>
+      <c r="H12" t="b">
+        <v>0</v>
+      </c>
+      <c r="I12" t="b">
+        <v>0</v>
+      </c>
+      <c r="J12"/>
+      <c r="K12"/>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="B13" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="C13" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="D13" t="b">
         <v>0</v>
@@ -1265,60 +1312,60 @@
         <v>1</v>
       </c>
       <c r="F13" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="G13" t="s">
-        <v>73</v>
-      </c>
-      <c r="H13"/>
-      <c r="I13"/>
-      <c r="J13" t="b">
-        <v>1</v>
-      </c>
-      <c r="K13" t="b">
-        <v>1</v>
-      </c>
+        <v>78</v>
+      </c>
+      <c r="H13" t="b">
+        <v>1</v>
+      </c>
+      <c r="I13" t="b">
+        <v>1</v>
+      </c>
+      <c r="J13"/>
+      <c r="K13"/>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>2</v>
+        <v>54</v>
       </c>
       <c r="B14" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C14" t="s">
-        <v>76</v>
+        <v>55</v>
       </c>
       <c r="D14" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E14" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F14" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="G14" t="s">
-        <v>73</v>
-      </c>
-      <c r="H14"/>
-      <c r="I14"/>
-      <c r="J14" t="b">
-        <v>0</v>
-      </c>
-      <c r="K14" t="b">
-        <v>0</v>
-      </c>
+        <v>82</v>
+      </c>
+      <c r="H14" t="b">
+        <v>1</v>
+      </c>
+      <c r="I14" t="b">
+        <v>1</v>
+      </c>
+      <c r="J14"/>
+      <c r="K14"/>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="B15" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="C15" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="D15" t="b">
         <v>0</v>
@@ -1327,122 +1374,122 @@
         <v>1</v>
       </c>
       <c r="F15" t="s">
-        <v>79</v>
+        <v>56</v>
       </c>
       <c r="G15" t="s">
-        <v>73</v>
-      </c>
-      <c r="H15"/>
-      <c r="I15"/>
-      <c r="J15" t="b">
-        <v>0</v>
-      </c>
-      <c r="K15" t="b">
-        <v>0</v>
-      </c>
+        <v>82</v>
+      </c>
+      <c r="H15" t="b">
+        <v>0</v>
+      </c>
+      <c r="I15" t="b">
+        <v>0</v>
+      </c>
+      <c r="J15"/>
+      <c r="K15"/>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>49</v>
+        <v>2</v>
       </c>
       <c r="B16" t="s">
-        <v>50</v>
+        <v>72</v>
       </c>
       <c r="C16" t="s">
-        <v>50</v>
+        <v>73</v>
       </c>
       <c r="D16" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E16" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F16" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="G16" t="s">
-        <v>80</v>
-      </c>
-      <c r="H16"/>
-      <c r="I16"/>
-      <c r="J16" t="b">
-        <v>0</v>
-      </c>
-      <c r="K16" t="b">
-        <v>0</v>
-      </c>
+        <v>82</v>
+      </c>
+      <c r="H16" t="b">
+        <v>0</v>
+      </c>
+      <c r="I16" t="b">
+        <v>0</v>
+      </c>
+      <c r="J16"/>
+      <c r="K16"/>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="B17" t="s">
+        <v>86</v>
+      </c>
+      <c r="C17" t="s">
+        <v>86</v>
+      </c>
+      <c r="D17" t="b">
+        <v>0</v>
+      </c>
+      <c r="E17" t="b">
+        <v>1</v>
+      </c>
+      <c r="F17" t="s">
+        <v>56</v>
+      </c>
+      <c r="G17" t="s">
         <v>82</v>
       </c>
-      <c r="C17" t="s">
-        <v>83</v>
-      </c>
-      <c r="D17" t="b">
-        <v>0</v>
-      </c>
-      <c r="E17" t="b">
-        <v>1</v>
-      </c>
-      <c r="F17" t="s">
-        <v>51</v>
-      </c>
-      <c r="G17" t="s">
-        <v>80</v>
-      </c>
-      <c r="H17"/>
-      <c r="I17"/>
-      <c r="J17" t="b">
-        <v>1</v>
-      </c>
-      <c r="K17" t="b">
-        <v>1</v>
-      </c>
+      <c r="H17" t="b">
+        <v>0</v>
+      </c>
+      <c r="I17" t="b">
+        <v>0</v>
+      </c>
+      <c r="J17"/>
+      <c r="K17"/>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>49</v>
+        <v>87</v>
       </c>
       <c r="B18" t="s">
-        <v>50</v>
+        <v>88</v>
       </c>
       <c r="C18" t="s">
-        <v>50</v>
+        <v>88</v>
       </c>
       <c r="D18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F18" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="G18" t="s">
-        <v>84</v>
-      </c>
-      <c r="H18"/>
-      <c r="I18"/>
-      <c r="J18" t="b">
-        <v>1</v>
-      </c>
-      <c r="K18" t="b">
-        <v>1</v>
-      </c>
+        <v>82</v>
+      </c>
+      <c r="H18" t="b">
+        <v>0</v>
+      </c>
+      <c r="I18" t="b">
+        <v>0</v>
+      </c>
+      <c r="J18"/>
+      <c r="K18"/>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="B19" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="C19" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="D19" t="b">
         <v>0</v>
@@ -1451,50 +1498,50 @@
         <v>1</v>
       </c>
       <c r="F19" t="s">
-        <v>51</v>
+        <v>90</v>
       </c>
       <c r="G19" t="s">
-        <v>84</v>
-      </c>
-      <c r="H19"/>
-      <c r="I19"/>
-      <c r="J19" t="b">
-        <v>0</v>
-      </c>
-      <c r="K19" t="b">
-        <v>0</v>
-      </c>
+        <v>82</v>
+      </c>
+      <c r="H19" t="b">
+        <v>0</v>
+      </c>
+      <c r="I19" t="b">
+        <v>0</v>
+      </c>
+      <c r="J19"/>
+      <c r="K19"/>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>2</v>
+        <v>54</v>
       </c>
       <c r="B20" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C20" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D20" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E20" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F20" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="G20" t="s">
-        <v>84</v>
-      </c>
-      <c r="H20"/>
-      <c r="I20"/>
-      <c r="J20" t="b">
-        <v>0</v>
-      </c>
-      <c r="K20" t="b">
-        <v>0</v>
-      </c>
+        <v>91</v>
+      </c>
+      <c r="H20" t="b">
+        <v>0</v>
+      </c>
+      <c r="I20" t="b">
+        <v>0</v>
+      </c>
+      <c r="J20"/>
+      <c r="K20"/>
     </row>
     <row r="21">
       <c r="A21" t="s">
@@ -1513,29 +1560,29 @@
         <v>1</v>
       </c>
       <c r="F21" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="G21" t="s">
-        <v>84</v>
-      </c>
-      <c r="H21"/>
-      <c r="I21"/>
-      <c r="J21" t="b">
-        <v>0</v>
-      </c>
-      <c r="K21" t="b">
-        <v>0</v>
-      </c>
+        <v>91</v>
+      </c>
+      <c r="H21" t="b">
+        <v>1</v>
+      </c>
+      <c r="I21" t="b">
+        <v>1</v>
+      </c>
+      <c r="J21"/>
+      <c r="K21"/>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>74</v>
+        <v>2</v>
       </c>
       <c r="B22" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C22" t="s">
-        <v>75</v>
+        <v>92</v>
       </c>
       <c r="D22" t="b">
         <v>0</v>
@@ -1544,29 +1591,29 @@
         <v>1</v>
       </c>
       <c r="F22" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="G22" t="s">
-        <v>84</v>
-      </c>
-      <c r="H22"/>
-      <c r="I22"/>
-      <c r="J22" t="b">
-        <v>0</v>
-      </c>
-      <c r="K22" t="b">
-        <v>0</v>
-      </c>
+        <v>91</v>
+      </c>
+      <c r="H22" t="b">
+        <v>0</v>
+      </c>
+      <c r="I22" t="b">
+        <v>0</v>
+      </c>
+      <c r="J22"/>
+      <c r="K22"/>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="B23" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="C23" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="D23" t="b">
         <v>0</v>
@@ -1575,19 +1622,50 @@
         <v>1</v>
       </c>
       <c r="F23" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="G23" t="s">
-        <v>84</v>
-      </c>
-      <c r="H23"/>
-      <c r="I23"/>
-      <c r="J23" t="b">
-        <v>0</v>
-      </c>
-      <c r="K23" t="b">
-        <v>0</v>
-      </c>
+        <v>91</v>
+      </c>
+      <c r="H23" t="b">
+        <v>0</v>
+      </c>
+      <c r="I23" t="b">
+        <v>0</v>
+      </c>
+      <c r="J23"/>
+      <c r="K23"/>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>96</v>
+      </c>
+      <c r="B24" t="s">
+        <v>97</v>
+      </c>
+      <c r="C24" t="s">
+        <v>98</v>
+      </c>
+      <c r="D24" t="b">
+        <v>1</v>
+      </c>
+      <c r="E24" t="b">
+        <v>0</v>
+      </c>
+      <c r="F24" t="s">
+        <v>56</v>
+      </c>
+      <c r="G24" t="s">
+        <v>99</v>
+      </c>
+      <c r="H24" t="b">
+        <v>1</v>
+      </c>
+      <c r="I24" t="b">
+        <v>1</v>
+      </c>
+      <c r="J24"/>
+      <c r="K24"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1631,19 +1709,19 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="B1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>85</v>
+      </c>
+      <c r="E1" t="s">
         <v>87</v>
-      </c>
-      <c r="E1" t="s">
-        <v>74</v>
       </c>
       <c r="F1" t="s">
         <v>89</v>
@@ -1651,42 +1729,42 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="B2" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
       <c r="C2" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="D2" t="s">
-        <v>94</v>
+        <v>103</v>
       </c>
       <c r="E2" t="s">
-        <v>95</v>
+        <v>104</v>
       </c>
       <c r="F2" t="s">
-        <v>96</v>
+        <v>105</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>97</v>
+        <v>106</v>
       </c>
       <c r="B3" t="s">
-        <v>98</v>
+        <v>107</v>
       </c>
       <c r="C3" t="s">
-        <v>99</v>
+        <v>108</v>
       </c>
       <c r="D3" t="s">
-        <v>94</v>
+        <v>103</v>
       </c>
       <c r="E3" t="s">
-        <v>100</v>
+        <v>109</v>
       </c>
       <c r="F3" t="s">
-        <v>101</v>
+        <v>110</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed typos and improved messages for yaml compiling
</commit_message>
<xml_diff>
--- a/emx/cosas-refs/cosasrefs.xlsx
+++ b/emx/cosas-refs/cosasrefs.xlsx
@@ -9,9 +9,7 @@
     <sheet name="packages" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="entities" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="attributes" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="cosasrefs_diagnostic_certainty" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="cosasrefs_lab_indications" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="cosasrefs_phenotypic_sex" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="cosasrefs_phenotypic_sex" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
 </workbook>
 </file>
@@ -2299,32 +2297,6 @@
     <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">

</xml_diff>

<commit_message>
fixed broken reference in cosasrefs
</commit_message>
<xml_diff>
--- a/emx/cosas-refs/cosasrefs.xlsx
+++ b/emx/cosas-refs/cosasrefs.xlsx
@@ -9,13 +9,13 @@
     <sheet name="packages" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="entities" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="attributes" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="cosasrefs_phenotypic_sex" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="cosasrefs_biological_sex" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="132">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -378,6 +378,39 @@
   </si>
   <si>
     <t xml:space="preserve">cosasrefs_test_genes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vrouw</t>
+  </si>
+  <si>
+    <t xml:space="preserve">female</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A biological sex quality inhering in an individual or a population that only produces gametes that can be fertilised by male gametes.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PATO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0000383</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://purl.obolibrary.org/obo/PATO_0000383</t>
+  </si>
+  <si>
+    <t xml:space="preserve">man</t>
+  </si>
+  <si>
+    <t xml:space="preserve">male</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A biological sex quality inhering in an individual or a population whose sex organs contain only male gametes.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0000384</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://purl.obolibrary.org/obo/PATO_0000384</t>
   </si>
 </sst>
 </file>
@@ -2264,7 +2297,68 @@
     <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>121</v>
+      </c>
+      <c r="B2" t="s">
+        <v>122</v>
+      </c>
+      <c r="C2" t="s">
+        <v>123</v>
+      </c>
+      <c r="D2" t="s">
+        <v>124</v>
+      </c>
+      <c r="E2" t="s">
+        <v>125</v>
+      </c>
+      <c r="F2" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>127</v>
+      </c>
+      <c r="B3" t="s">
+        <v>128</v>
+      </c>
+      <c r="C3" t="s">
+        <v>129</v>
+      </c>
+      <c r="D3" t="s">
+        <v>124</v>
+      </c>
+      <c r="E3" t="s">
+        <v>130</v>
+      </c>
+      <c r="F3" t="s">
+        <v>131</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>

</xml_diff>

<commit_message>
fix: change variable names and integrated cineas-hpo mappings (#3)
</commit_message>
<xml_diff>
--- a/emx/cosas-refs/cosasrefs.xlsx
+++ b/emx/cosas-refs/cosasrefs.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="159">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -35,7 +35,7 @@
     <t xml:space="preserve">COSAS References</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference tables for COSAS (v0.9021, 2021-08-30)</t>
+    <t xml:space="preserve">Reference tables for COSAS (v0.9022, 2021-09-01)</t>
   </si>
   <si>
     <t xml:space="preserve">label-nl</t>
@@ -176,6 +176,9 @@
     <t xml:space="preserve">labelAttribute</t>
   </si>
   <si>
+    <t xml:space="preserve">refEntity</t>
+  </si>
+  <si>
     <t xml:space="preserve">id</t>
   </si>
   <si>
@@ -224,25 +227,19 @@
     <t xml:space="preserve">cosasrefs_diagnoses</t>
   </si>
   <si>
-    <t xml:space="preserve">cineasCode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CINEAS code</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Diagnostic code (e.g., 12345)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Diagnostische code (bijv, 12345)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cineasDescription</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Diagnosis</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Diagnose</t>
+    <t xml:space="preserve">Cineas code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cineas description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hpo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mref</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cosasrefs_phenotype</t>
   </si>
   <si>
     <t xml:space="preserve">cosasrefs_inclusionStatus</t>
@@ -297,9 +294,6 @@
   </si>
   <si>
     <t xml:space="preserve">FairGenomes iri</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cosasrefs_phenotype</t>
   </si>
   <si>
     <t xml:space="preserve">text</t>
@@ -1094,18 +1088,21 @@
         <v>2</v>
       </c>
       <c r="K1" t="s">
+        <v>52</v>
+      </c>
+      <c r="L1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D2" t="b">
         <v>1</v>
@@ -1114,10 +1111,10 @@
         <v>0</v>
       </c>
       <c r="F2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H2" t="b">
         <v>0</v>
@@ -1127,28 +1124,29 @@
       </c>
       <c r="J2"/>
       <c r="K2"/>
+      <c r="L2"/>
     </row>
     <row r="3">
       <c r="A3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D3" t="b">
+        <v>0</v>
+      </c>
+      <c r="E3" t="b">
+        <v>1</v>
+      </c>
+      <c r="F3" t="s">
+        <v>55</v>
+      </c>
+      <c r="G3" t="s">
         <v>56</v>
-      </c>
-      <c r="B3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D3" t="b">
-        <v>0</v>
-      </c>
-      <c r="E3" t="b">
-        <v>1</v>
-      </c>
-      <c r="F3" t="s">
-        <v>54</v>
-      </c>
-      <c r="G3" t="s">
-        <v>55</v>
       </c>
       <c r="H3" t="b">
         <v>1</v>
@@ -1158,16 +1156,17 @@
       </c>
       <c r="J3"/>
       <c r="K3"/>
+      <c r="L3"/>
     </row>
     <row r="4">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C4" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D4" t="b">
         <v>0</v>
@@ -1176,10 +1175,10 @@
         <v>1</v>
       </c>
       <c r="F4" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G4" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H4" t="b">
         <v>0</v>
@@ -1189,16 +1188,17 @@
       </c>
       <c r="J4"/>
       <c r="K4"/>
+      <c r="L4"/>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B5" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C5" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D5" t="b">
         <v>0</v>
@@ -1207,10 +1207,10 @@
         <v>1</v>
       </c>
       <c r="F5" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G5" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H5" t="b">
         <v>0</v>
@@ -1220,16 +1220,17 @@
       </c>
       <c r="J5"/>
       <c r="K5"/>
+      <c r="L5"/>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B6" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C6" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D6" t="b">
         <v>0</v>
@@ -1238,10 +1239,10 @@
         <v>1</v>
       </c>
       <c r="F6" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G6" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H6" t="b">
         <v>0</v>
@@ -1251,16 +1252,17 @@
       </c>
       <c r="J6"/>
       <c r="K6"/>
+      <c r="L6"/>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B7" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C7" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D7" t="b">
         <v>0</v>
@@ -1269,10 +1271,10 @@
         <v>1</v>
       </c>
       <c r="F7" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="G7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H7" t="b">
         <v>0</v>
@@ -1282,16 +1284,17 @@
       </c>
       <c r="J7"/>
       <c r="K7"/>
+      <c r="L7"/>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B8" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C8" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D8" t="b">
         <v>1</v>
@@ -1300,10 +1303,10 @@
         <v>0</v>
       </c>
       <c r="F8" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H8" t="b">
         <v>1</v>
@@ -1313,28 +1316,29 @@
       </c>
       <c r="J8"/>
       <c r="K8"/>
+      <c r="L8"/>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B9" t="s">
+        <v>67</v>
+      </c>
+      <c r="C9" t="s">
+        <v>67</v>
+      </c>
+      <c r="D9" t="b">
+        <v>0</v>
+      </c>
+      <c r="E9" t="b">
+        <v>1</v>
+      </c>
+      <c r="F9" t="s">
+        <v>55</v>
+      </c>
+      <c r="G9" t="s">
         <v>66</v>
-      </c>
-      <c r="C9" t="s">
-        <v>66</v>
-      </c>
-      <c r="D9" t="b">
-        <v>0</v>
-      </c>
-      <c r="E9" t="b">
-        <v>1</v>
-      </c>
-      <c r="F9" t="s">
-        <v>54</v>
-      </c>
-      <c r="G9" t="s">
-        <v>65</v>
       </c>
       <c r="H9" t="b">
         <v>0</v>
@@ -1344,16 +1348,17 @@
       </c>
       <c r="J9"/>
       <c r="K9"/>
+      <c r="L9"/>
     </row>
     <row r="10">
       <c r="A10" t="s">
         <v>2</v>
       </c>
       <c r="B10" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C10" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D10" t="b">
         <v>0</v>
@@ -1362,10 +1367,10 @@
         <v>1</v>
       </c>
       <c r="F10" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G10" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H10" t="b">
         <v>0</v>
@@ -1375,16 +1380,17 @@
       </c>
       <c r="J10"/>
       <c r="K10"/>
+      <c r="L10"/>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B11" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C11" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D11" t="b">
         <v>0</v>
@@ -1393,10 +1399,10 @@
         <v>1</v>
       </c>
       <c r="F11" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G11" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H11" t="b">
         <v>0</v>
@@ -1406,16 +1412,17 @@
       </c>
       <c r="J11"/>
       <c r="K11"/>
+      <c r="L11"/>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B12" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C12" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D12" t="b">
         <v>0</v>
@@ -1424,10 +1431,10 @@
         <v>1</v>
       </c>
       <c r="F12" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G12" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H12" t="b">
         <v>0</v>
@@ -1437,16 +1444,17 @@
       </c>
       <c r="J12"/>
       <c r="K12"/>
+      <c r="L12"/>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B13" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C13" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D13" t="b">
         <v>0</v>
@@ -1455,10 +1463,10 @@
         <v>1</v>
       </c>
       <c r="F13" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="G13" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H13" t="b">
         <v>0</v>
@@ -1468,17 +1476,14 @@
       </c>
       <c r="J13"/>
       <c r="K13"/>
+      <c r="L13"/>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>52</v>
-      </c>
-      <c r="B14" t="s">
         <v>53</v>
       </c>
-      <c r="C14" t="s">
-        <v>53</v>
-      </c>
+      <c r="B14"/>
+      <c r="C14"/>
       <c r="D14" t="b">
         <v>1</v>
       </c>
@@ -1486,65 +1491,57 @@
         <v>0</v>
       </c>
       <c r="F14" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G14" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="H14" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I14" t="b">
         <v>0</v>
       </c>
       <c r="J14"/>
       <c r="K14"/>
+      <c r="L14"/>
     </row>
     <row r="15">
       <c r="A15" t="s">
+        <v>62</v>
+      </c>
+      <c r="B15"/>
+      <c r="C15"/>
+      <c r="D15" t="b">
+        <v>0</v>
+      </c>
+      <c r="E15" t="b">
+        <v>1</v>
+      </c>
+      <c r="F15" t="s">
+        <v>55</v>
+      </c>
+      <c r="G15" t="s">
         <v>68</v>
       </c>
-      <c r="B15" t="s">
+      <c r="H15" t="b">
+        <v>0</v>
+      </c>
+      <c r="I15" t="b">
+        <v>1</v>
+      </c>
+      <c r="J15" t="s">
         <v>69</v>
       </c>
-      <c r="C15" t="s">
-        <v>69</v>
-      </c>
-      <c r="D15" t="b">
-        <v>0</v>
-      </c>
-      <c r="E15" t="b">
-        <v>1</v>
-      </c>
-      <c r="F15" t="s">
-        <v>54</v>
-      </c>
-      <c r="G15" t="s">
-        <v>67</v>
-      </c>
-      <c r="H15" t="b">
-        <v>0</v>
-      </c>
-      <c r="I15" t="b">
-        <v>1</v>
-      </c>
-      <c r="J15" t="s">
-        <v>70</v>
-      </c>
-      <c r="K15" t="s">
-        <v>71</v>
-      </c>
+      <c r="K15"/>
+      <c r="L15"/>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>72</v>
-      </c>
-      <c r="B16" t="s">
-        <v>73</v>
-      </c>
-      <c r="C16" t="s">
-        <v>74</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="B16"/>
+      <c r="C16"/>
       <c r="D16" t="b">
         <v>0</v>
       </c>
@@ -1552,10 +1549,10 @@
         <v>1</v>
       </c>
       <c r="F16" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G16" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="H16" t="b">
         <v>0</v>
@@ -1565,48 +1562,44 @@
       </c>
       <c r="J16"/>
       <c r="K16"/>
+      <c r="L16"/>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>52</v>
-      </c>
-      <c r="B17" t="s">
-        <v>53</v>
-      </c>
-      <c r="C17" t="s">
-        <v>53</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="B17"/>
+      <c r="C17"/>
       <c r="D17" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E17" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F17" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G17" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="H17" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I17" t="b">
-        <v>0</v>
-      </c>
-      <c r="J17"/>
+        <v>1</v>
+      </c>
+      <c r="J17" t="s">
+        <v>70</v>
+      </c>
       <c r="K17"/>
+      <c r="L17"/>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>56</v>
-      </c>
-      <c r="B18" t="s">
-        <v>66</v>
-      </c>
-      <c r="C18" t="s">
-        <v>66</v>
-      </c>
+        <v>71</v>
+      </c>
+      <c r="B18"/>
+      <c r="C18"/>
       <c r="D18" t="b">
         <v>0</v>
       </c>
@@ -1614,10 +1607,10 @@
         <v>1</v>
       </c>
       <c r="F18" t="s">
-        <v>54</v>
+        <v>72</v>
       </c>
       <c r="G18" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="H18" t="b">
         <v>0</v>
@@ -1625,34 +1618,33 @@
       <c r="I18" t="b">
         <v>0</v>
       </c>
-      <c r="J18" t="s">
-        <v>76</v>
-      </c>
+      <c r="J18"/>
       <c r="K18" t="s">
-        <v>76</v>
-      </c>
+        <v>73</v>
+      </c>
+      <c r="L18"/>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>2</v>
+        <v>53</v>
       </c>
       <c r="B19" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C19" t="s">
-        <v>77</v>
+        <v>54</v>
       </c>
       <c r="D19" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E19" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F19" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G19" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H19" t="b">
         <v>0</v>
@@ -1660,22 +1652,19 @@
       <c r="I19" t="b">
         <v>0</v>
       </c>
-      <c r="J19" t="s">
-        <v>78</v>
-      </c>
-      <c r="K19" t="s">
-        <v>79</v>
-      </c>
+      <c r="J19"/>
+      <c r="K19"/>
+      <c r="L19"/>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B20" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
       <c r="C20" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
       <c r="D20" t="b">
         <v>0</v>
@@ -1684,33 +1673,34 @@
         <v>1</v>
       </c>
       <c r="F20" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G20" t="s">
+        <v>74</v>
+      </c>
+      <c r="H20" t="b">
+        <v>0</v>
+      </c>
+      <c r="I20" t="b">
+        <v>0</v>
+      </c>
+      <c r="J20" t="s">
         <v>75</v>
       </c>
-      <c r="H20" t="b">
-        <v>0</v>
-      </c>
-      <c r="I20" t="b">
-        <v>0</v>
-      </c>
-      <c r="J20" t="s">
-        <v>81</v>
-      </c>
-      <c r="K20" t="s">
-        <v>81</v>
+      <c r="K20"/>
+      <c r="L20" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>61</v>
+        <v>2</v>
       </c>
       <c r="B21" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C21" t="s">
-        <v>62</v>
+        <v>76</v>
       </c>
       <c r="D21" t="b">
         <v>0</v>
@@ -1719,10 +1709,10 @@
         <v>1</v>
       </c>
       <c r="F21" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G21" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H21" t="b">
         <v>0</v>
@@ -1731,21 +1721,22 @@
         <v>0</v>
       </c>
       <c r="J21" t="s">
-        <v>82</v>
-      </c>
-      <c r="K21" t="s">
-        <v>82</v>
+        <v>77</v>
+      </c>
+      <c r="K21"/>
+      <c r="L21" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B22" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C22" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="D22" t="b">
         <v>0</v>
@@ -1754,10 +1745,10 @@
         <v>1</v>
       </c>
       <c r="F22" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="G22" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H22" t="b">
         <v>0</v>
@@ -1766,33 +1757,34 @@
         <v>0</v>
       </c>
       <c r="J22" t="s">
-        <v>84</v>
-      </c>
-      <c r="K22" t="s">
-        <v>84</v>
+        <v>80</v>
+      </c>
+      <c r="K22"/>
+      <c r="L22" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="B23" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="C23" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="D23" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E23" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F23" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G23" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="H23" t="b">
         <v>0</v>
@@ -1800,18 +1792,23 @@
       <c r="I23" t="b">
         <v>0</v>
       </c>
-      <c r="J23"/>
+      <c r="J23" t="s">
+        <v>81</v>
+      </c>
       <c r="K23"/>
+      <c r="L23" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="B24" t="s">
-        <v>66</v>
+        <v>82</v>
       </c>
       <c r="C24" t="s">
-        <v>66</v>
+        <v>82</v>
       </c>
       <c r="D24" t="b">
         <v>0</v>
@@ -1820,41 +1817,46 @@
         <v>1</v>
       </c>
       <c r="F24" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="G24" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="H24" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I24" t="b">
-        <v>1</v>
-      </c>
-      <c r="J24"/>
+        <v>0</v>
+      </c>
+      <c r="J24" t="s">
+        <v>83</v>
+      </c>
       <c r="K24"/>
+      <c r="L24" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>2</v>
+        <v>53</v>
       </c>
       <c r="B25" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C25" t="s">
-        <v>77</v>
+        <v>54</v>
       </c>
       <c r="D25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F25" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G25" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H25" t="b">
         <v>0</v>
@@ -1862,22 +1864,19 @@
       <c r="I25" t="b">
         <v>0</v>
       </c>
-      <c r="J25" t="s">
-        <v>78</v>
-      </c>
-      <c r="K25" t="s">
-        <v>79</v>
-      </c>
+      <c r="J25"/>
+      <c r="K25"/>
+      <c r="L25"/>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B26" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
       <c r="C26" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
       <c r="D26" t="b">
         <v>0</v>
@@ -1886,33 +1885,30 @@
         <v>1</v>
       </c>
       <c r="F26" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G26" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H26" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I26" t="b">
-        <v>0</v>
-      </c>
-      <c r="J26" t="s">
-        <v>81</v>
-      </c>
-      <c r="K26" t="s">
-        <v>81</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="J26"/>
+      <c r="K26"/>
+      <c r="L26"/>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>61</v>
+        <v>2</v>
       </c>
       <c r="B27" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C27" t="s">
-        <v>62</v>
+        <v>76</v>
       </c>
       <c r="D27" t="b">
         <v>0</v>
@@ -1921,10 +1917,10 @@
         <v>1</v>
       </c>
       <c r="F27" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G27" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H27" t="b">
         <v>0</v>
@@ -1933,21 +1929,22 @@
         <v>0</v>
       </c>
       <c r="J27" t="s">
-        <v>82</v>
-      </c>
-      <c r="K27" t="s">
-        <v>82</v>
+        <v>77</v>
+      </c>
+      <c r="K27"/>
+      <c r="L27" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B28" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C28" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="D28" t="b">
         <v>0</v>
@@ -1956,10 +1953,10 @@
         <v>1</v>
       </c>
       <c r="F28" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="G28" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H28" t="b">
         <v>0</v>
@@ -1968,33 +1965,34 @@
         <v>0</v>
       </c>
       <c r="J28" t="s">
-        <v>84</v>
-      </c>
-      <c r="K28" t="s">
-        <v>84</v>
+        <v>80</v>
+      </c>
+      <c r="K28"/>
+      <c r="L28" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="B29" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="C29" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="D29" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E29" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F29" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G29" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H29" t="b">
         <v>0</v>
@@ -2002,18 +2000,23 @@
       <c r="I29" t="b">
         <v>0</v>
       </c>
-      <c r="J29"/>
+      <c r="J29" t="s">
+        <v>81</v>
+      </c>
       <c r="K29"/>
+      <c r="L29" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>87</v>
+        <v>64</v>
       </c>
       <c r="B30" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="C30" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="D30" t="b">
         <v>0</v>
@@ -2022,41 +2025,46 @@
         <v>1</v>
       </c>
       <c r="F30" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="G30" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H30" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I30" t="b">
-        <v>1</v>
-      </c>
-      <c r="J30"/>
+        <v>0</v>
+      </c>
+      <c r="J30" t="s">
+        <v>83</v>
+      </c>
       <c r="K30"/>
+      <c r="L30" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B31" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="C31" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="D31" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E31" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F31" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G31" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H31" t="b">
         <v>0</v>
@@ -2064,22 +2072,19 @@
       <c r="I31" t="b">
         <v>0</v>
       </c>
-      <c r="J31" t="s">
-        <v>90</v>
-      </c>
-      <c r="K31" t="s">
-        <v>91</v>
-      </c>
+      <c r="J31"/>
+      <c r="K31"/>
+      <c r="L31"/>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>2</v>
+        <v>86</v>
       </c>
       <c r="B32" t="s">
-        <v>57</v>
+        <v>87</v>
       </c>
       <c r="C32" t="s">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="D32" t="b">
         <v>0</v>
@@ -2088,33 +2093,30 @@
         <v>1</v>
       </c>
       <c r="F32" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G32" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H32" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I32" t="b">
-        <v>0</v>
-      </c>
-      <c r="J32" t="s">
-        <v>78</v>
-      </c>
-      <c r="K32" t="s">
-        <v>79</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="J32"/>
+      <c r="K32"/>
+      <c r="L32"/>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B33" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
       <c r="C33" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
       <c r="D33" t="b">
         <v>0</v>
@@ -2123,10 +2125,10 @@
         <v>1</v>
       </c>
       <c r="F33" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G33" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H33" t="b">
         <v>0</v>
@@ -2135,21 +2137,22 @@
         <v>0</v>
       </c>
       <c r="J33" t="s">
-        <v>81</v>
-      </c>
-      <c r="K33" t="s">
-        <v>81</v>
+        <v>89</v>
+      </c>
+      <c r="K33"/>
+      <c r="L33" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>61</v>
+        <v>2</v>
       </c>
       <c r="B34" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C34" t="s">
-        <v>62</v>
+        <v>76</v>
       </c>
       <c r="D34" t="b">
         <v>0</v>
@@ -2158,10 +2161,10 @@
         <v>1</v>
       </c>
       <c r="F34" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G34" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H34" t="b">
         <v>0</v>
@@ -2170,21 +2173,22 @@
         <v>0</v>
       </c>
       <c r="J34" t="s">
-        <v>82</v>
-      </c>
-      <c r="K34" t="s">
-        <v>82</v>
+        <v>77</v>
+      </c>
+      <c r="K34"/>
+      <c r="L34" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B35" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C35" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="D35" t="b">
         <v>0</v>
@@ -2193,10 +2197,10 @@
         <v>1</v>
       </c>
       <c r="F35" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="G35" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H35" t="b">
         <v>0</v>
@@ -2205,18 +2209,23 @@
         <v>0</v>
       </c>
       <c r="J35" t="s">
-        <v>92</v>
-      </c>
-      <c r="K35" t="s">
-        <v>92</v>
+        <v>80</v>
+      </c>
+      <c r="K35"/>
+      <c r="L35" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>56</v>
-      </c>
-      <c r="B36"/>
-      <c r="C36"/>
+        <v>62</v>
+      </c>
+      <c r="B36" t="s">
+        <v>63</v>
+      </c>
+      <c r="C36" t="s">
+        <v>63</v>
+      </c>
       <c r="D36" t="b">
         <v>0</v>
       </c>
@@ -2224,26 +2233,35 @@
         <v>1</v>
       </c>
       <c r="F36" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G36" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="H36" t="b">
         <v>0</v>
       </c>
       <c r="I36" t="b">
-        <v>1</v>
-      </c>
-      <c r="J36"/>
+        <v>0</v>
+      </c>
+      <c r="J36" t="s">
+        <v>81</v>
+      </c>
       <c r="K36"/>
+      <c r="L36" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>2</v>
-      </c>
-      <c r="B37"/>
-      <c r="C37"/>
+        <v>64</v>
+      </c>
+      <c r="B37" t="s">
+        <v>82</v>
+      </c>
+      <c r="C37" t="s">
+        <v>82</v>
+      </c>
       <c r="D37" t="b">
         <v>0</v>
       </c>
@@ -2251,10 +2269,10 @@
         <v>1</v>
       </c>
       <c r="F37" t="s">
-        <v>94</v>
+        <v>65</v>
       </c>
       <c r="G37" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="H37" t="b">
         <v>0</v>
@@ -2262,12 +2280,17 @@
       <c r="I37" t="b">
         <v>0</v>
       </c>
-      <c r="J37"/>
+      <c r="J37" t="s">
+        <v>91</v>
+      </c>
       <c r="K37"/>
+      <c r="L37" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B38"/>
       <c r="C38"/>
@@ -2278,10 +2301,10 @@
         <v>1</v>
       </c>
       <c r="F38" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G38" t="s">
-        <v>93</v>
+        <v>73</v>
       </c>
       <c r="H38" t="b">
         <v>0</v>
@@ -2291,37 +2314,39 @@
       </c>
       <c r="J38"/>
       <c r="K38"/>
+      <c r="L38"/>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>61</v>
+        <v>2</v>
       </c>
       <c r="B39"/>
       <c r="C39"/>
       <c r="D39" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E39" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F39" t="s">
-        <v>54</v>
+        <v>92</v>
       </c>
       <c r="G39" t="s">
-        <v>93</v>
+        <v>73</v>
       </c>
       <c r="H39" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I39" t="b">
         <v>0</v>
       </c>
       <c r="J39"/>
       <c r="K39"/>
+      <c r="L39"/>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B40"/>
       <c r="C40"/>
@@ -2332,10 +2357,10 @@
         <v>1</v>
       </c>
       <c r="F40" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G40" t="s">
-        <v>93</v>
+        <v>73</v>
       </c>
       <c r="H40" t="b">
         <v>0</v>
@@ -2345,17 +2370,14 @@
       </c>
       <c r="J40"/>
       <c r="K40"/>
+      <c r="L40"/>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>52</v>
-      </c>
-      <c r="B41" t="s">
-        <v>53</v>
-      </c>
-      <c r="C41" t="s">
-        <v>53</v>
-      </c>
+        <v>62</v>
+      </c>
+      <c r="B41"/>
+      <c r="C41"/>
       <c r="D41" t="b">
         <v>1</v>
       </c>
@@ -2363,30 +2385,27 @@
         <v>0</v>
       </c>
       <c r="F41" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G41" t="s">
-        <v>95</v>
+        <v>73</v>
       </c>
       <c r="H41" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I41" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J41"/>
       <c r="K41"/>
+      <c r="L41"/>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>61</v>
-      </c>
-      <c r="B42" t="s">
-        <v>62</v>
-      </c>
-      <c r="C42" t="s">
-        <v>62</v>
-      </c>
+        <v>64</v>
+      </c>
+      <c r="B42"/>
+      <c r="C42"/>
       <c r="D42" t="b">
         <v>0</v>
       </c>
@@ -2394,41 +2413,42 @@
         <v>1</v>
       </c>
       <c r="F42" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G42" t="s">
-        <v>95</v>
+        <v>73</v>
       </c>
       <c r="H42" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I42" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J42"/>
       <c r="K42"/>
+      <c r="L42"/>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>2</v>
+        <v>53</v>
       </c>
       <c r="B43" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C43" t="s">
-        <v>77</v>
+        <v>54</v>
       </c>
       <c r="D43" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E43" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F43" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G43" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="H43" t="b">
         <v>0</v>
@@ -2438,16 +2458,17 @@
       </c>
       <c r="J43"/>
       <c r="K43"/>
+      <c r="L43"/>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>1</v>
+        <v>62</v>
       </c>
       <c r="B44" t="s">
-        <v>96</v>
+        <v>63</v>
       </c>
       <c r="C44" t="s">
-        <v>96</v>
+        <v>63</v>
       </c>
       <c r="D44" t="b">
         <v>0</v>
@@ -2456,29 +2477,30 @@
         <v>1</v>
       </c>
       <c r="F44" t="s">
-        <v>94</v>
+        <v>55</v>
       </c>
       <c r="G44" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="H44" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I44" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J44"/>
       <c r="K44"/>
+      <c r="L44"/>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>97</v>
+        <v>2</v>
       </c>
       <c r="B45" t="s">
-        <v>98</v>
+        <v>58</v>
       </c>
       <c r="C45" t="s">
-        <v>98</v>
+        <v>76</v>
       </c>
       <c r="D45" t="b">
         <v>0</v>
@@ -2487,10 +2509,10 @@
         <v>1</v>
       </c>
       <c r="F45" t="s">
-        <v>94</v>
+        <v>55</v>
       </c>
       <c r="G45" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="H45" t="b">
         <v>0</v>
@@ -2500,16 +2522,17 @@
       </c>
       <c r="J45"/>
       <c r="K45"/>
+      <c r="L45"/>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>99</v>
+        <v>1</v>
       </c>
       <c r="B46" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="C46" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="D46" t="b">
         <v>0</v>
@@ -2518,10 +2541,10 @@
         <v>1</v>
       </c>
       <c r="F46" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="G46" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="H46" t="b">
         <v>0</v>
@@ -2531,6 +2554,71 @@
       </c>
       <c r="J46"/>
       <c r="K46"/>
+      <c r="L46"/>
+    </row>
+    <row r="47">
+      <c r="A47" t="s">
+        <v>95</v>
+      </c>
+      <c r="B47" t="s">
+        <v>96</v>
+      </c>
+      <c r="C47" t="s">
+        <v>96</v>
+      </c>
+      <c r="D47" t="b">
+        <v>0</v>
+      </c>
+      <c r="E47" t="b">
+        <v>1</v>
+      </c>
+      <c r="F47" t="s">
+        <v>92</v>
+      </c>
+      <c r="G47" t="s">
+        <v>93</v>
+      </c>
+      <c r="H47" t="b">
+        <v>0</v>
+      </c>
+      <c r="I47" t="b">
+        <v>0</v>
+      </c>
+      <c r="J47"/>
+      <c r="K47"/>
+      <c r="L47"/>
+    </row>
+    <row r="48">
+      <c r="A48" t="s">
+        <v>97</v>
+      </c>
+      <c r="B48" t="s">
+        <v>98</v>
+      </c>
+      <c r="C48" t="s">
+        <v>98</v>
+      </c>
+      <c r="D48" t="b">
+        <v>0</v>
+      </c>
+      <c r="E48" t="b">
+        <v>1</v>
+      </c>
+      <c r="F48" t="s">
+        <v>92</v>
+      </c>
+      <c r="G48" t="s">
+        <v>93</v>
+      </c>
+      <c r="H48" t="b">
+        <v>0</v>
+      </c>
+      <c r="I48" t="b">
+        <v>0</v>
+      </c>
+      <c r="J48"/>
+      <c r="K48"/>
+      <c r="L48"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2548,102 +2636,102 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="F1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C2" t="s">
         <v>101</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
         <v>102</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
+        <v>99</v>
+      </c>
+      <c r="F2" t="s">
         <v>103</v>
-      </c>
-      <c r="D2" t="s">
-        <v>104</v>
-      </c>
-      <c r="E2" t="s">
-        <v>101</v>
-      </c>
-      <c r="F2" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
+        <v>104</v>
+      </c>
+      <c r="B3" t="s">
+        <v>105</v>
+      </c>
+      <c r="C3" t="s">
         <v>106</v>
       </c>
-      <c r="B3" t="s">
+      <c r="D3" t="s">
         <v>107</v>
       </c>
-      <c r="C3" t="s">
+      <c r="E3" t="s">
         <v>108</v>
       </c>
-      <c r="D3" t="s">
+      <c r="F3" t="s">
         <v>109</v>
-      </c>
-      <c r="E3" t="s">
-        <v>110</v>
-      </c>
-      <c r="F3" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
+        <v>110</v>
+      </c>
+      <c r="B4" t="s">
+        <v>111</v>
+      </c>
+      <c r="C4" t="s">
         <v>112</v>
       </c>
-      <c r="B4" t="s">
+      <c r="D4" t="s">
+        <v>107</v>
+      </c>
+      <c r="E4" t="s">
         <v>113</v>
       </c>
-      <c r="C4" t="s">
+      <c r="F4" t="s">
         <v>114</v>
-      </c>
-      <c r="D4" t="s">
-        <v>109</v>
-      </c>
-      <c r="E4" t="s">
-        <v>115</v>
-      </c>
-      <c r="F4" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
+        <v>115</v>
+      </c>
+      <c r="B5" t="s">
+        <v>116</v>
+      </c>
+      <c r="C5" t="s">
         <v>117</v>
       </c>
-      <c r="B5" t="s">
+      <c r="D5" t="s">
+        <v>107</v>
+      </c>
+      <c r="E5" t="s">
         <v>118</v>
       </c>
-      <c r="C5" t="s">
+      <c r="F5" t="s">
         <v>119</v>
-      </c>
-      <c r="D5" t="s">
-        <v>109</v>
-      </c>
-      <c r="E5" t="s">
-        <v>120</v>
-      </c>
-      <c r="F5" t="s">
-        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -2662,82 +2750,82 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="F1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B2" t="s">
+        <v>120</v>
+      </c>
+      <c r="C2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D2" t="s">
         <v>122</v>
       </c>
-      <c r="B2" t="s">
-        <v>122</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>123</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>124</v>
-      </c>
-      <c r="E2" t="s">
-        <v>125</v>
-      </c>
-      <c r="F2" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
+        <v>125</v>
+      </c>
+      <c r="B3" t="s">
+        <v>125</v>
+      </c>
+      <c r="C3" t="s">
+        <v>126</v>
+      </c>
+      <c r="D3" t="s">
+        <v>122</v>
+      </c>
+      <c r="E3" t="s">
         <v>127</v>
       </c>
-      <c r="B3" t="s">
-        <v>127</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="F3" t="s">
         <v>128</v>
-      </c>
-      <c r="D3" t="s">
-        <v>124</v>
-      </c>
-      <c r="E3" t="s">
-        <v>129</v>
-      </c>
-      <c r="F3" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
+        <v>115</v>
+      </c>
+      <c r="B4" t="s">
+        <v>115</v>
+      </c>
+      <c r="C4" t="s">
         <v>117</v>
       </c>
-      <c r="B4" t="s">
-        <v>117</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
+        <v>107</v>
+      </c>
+      <c r="E4" t="s">
+        <v>118</v>
+      </c>
+      <c r="F4" t="s">
         <v>119</v>
-      </c>
-      <c r="D4" t="s">
-        <v>109</v>
-      </c>
-      <c r="E4" t="s">
-        <v>120</v>
-      </c>
-      <c r="F4" t="s">
-        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -2756,102 +2844,102 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="F1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
+        <v>129</v>
+      </c>
+      <c r="B2" t="s">
+        <v>130</v>
+      </c>
+      <c r="C2" t="s">
         <v>131</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
+        <v>102</v>
+      </c>
+      <c r="E2" t="s">
         <v>132</v>
       </c>
-      <c r="C2" t="s">
+      <c r="F2" t="s">
         <v>133</v>
-      </c>
-      <c r="D2" t="s">
-        <v>104</v>
-      </c>
-      <c r="E2" t="s">
-        <v>134</v>
-      </c>
-      <c r="F2" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
+        <v>134</v>
+      </c>
+      <c r="B3" t="s">
+        <v>135</v>
+      </c>
+      <c r="C3" t="s">
         <v>136</v>
       </c>
-      <c r="B3" t="s">
+      <c r="D3" t="s">
+        <v>102</v>
+      </c>
+      <c r="E3" t="s">
         <v>137</v>
       </c>
-      <c r="C3" t="s">
+      <c r="F3" t="s">
         <v>138</v>
-      </c>
-      <c r="D3" t="s">
-        <v>104</v>
-      </c>
-      <c r="E3" t="s">
-        <v>139</v>
-      </c>
-      <c r="F3" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
+        <v>139</v>
+      </c>
+      <c r="B4" t="s">
+        <v>140</v>
+      </c>
+      <c r="C4" t="s">
         <v>141</v>
       </c>
-      <c r="B4" t="s">
+      <c r="D4" t="s">
+        <v>102</v>
+      </c>
+      <c r="E4" t="s">
         <v>142</v>
       </c>
-      <c r="C4" t="s">
+      <c r="F4" t="s">
         <v>143</v>
-      </c>
-      <c r="D4" t="s">
-        <v>104</v>
-      </c>
-      <c r="E4" t="s">
-        <v>144</v>
-      </c>
-      <c r="F4" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
+        <v>115</v>
+      </c>
+      <c r="B5" t="s">
+        <v>116</v>
+      </c>
+      <c r="C5" t="s">
         <v>117</v>
       </c>
-      <c r="B5" t="s">
+      <c r="D5" t="s">
+        <v>107</v>
+      </c>
+      <c r="E5" t="s">
         <v>118</v>
       </c>
-      <c r="C5" t="s">
+      <c r="F5" t="s">
         <v>119</v>
-      </c>
-      <c r="D5" t="s">
-        <v>109</v>
-      </c>
-      <c r="E5" t="s">
-        <v>120</v>
-      </c>
-      <c r="F5" t="s">
-        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -2870,162 +2958,162 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="F1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
+        <v>144</v>
+      </c>
+      <c r="B2" t="s">
+        <v>145</v>
+      </c>
+      <c r="C2" t="s">
         <v>146</v>
       </c>
-      <c r="B2" t="s">
-        <v>147</v>
-      </c>
-      <c r="C2" t="s">
-        <v>148</v>
-      </c>
       <c r="D2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="F2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="F3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B4" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C4" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D4" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E4" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="F4" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B5" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C5" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D5" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E5" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="F5" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B6" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C6" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D6" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E6" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="F6" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B7" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C7" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D7" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E7" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="F7" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B8" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C8" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D8" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E8" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="F8" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
   </sheetData>

</xml_diff>